<commit_message>
final changes to data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szelenka/Documents/_svn/github/shrink_linalg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C42D7-BD7B-2044-81D6-5610AD5BD216}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BD427A-4378-134C-9E53-9C4F3266FDC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="1340" windowWidth="27640" windowHeight="16940" xr2:uid="{2189CFDE-40AF-8844-BA9C-6D3E4DAA80A6}"/>
+    <workbookView xWindow="3920" yWindow="2400" windowWidth="27640" windowHeight="16940" xr2:uid="{2189CFDE-40AF-8844-BA9C-6D3E4DAA80A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>CFLAG</t>
   </si>
@@ -179,6 +179,27 @@
   </si>
   <si>
     <t>31M</t>
+  </si>
+  <si>
+    <t>17M</t>
+  </si>
+  <si>
+    <t>57M</t>
+  </si>
+  <si>
+    <t>321M</t>
+  </si>
+  <si>
+    <t>546MB</t>
+  </si>
+  <si>
+    <t>w/alpine</t>
+  </si>
+  <si>
+    <t>w/debian-slim</t>
+  </si>
+  <si>
+    <t>334M</t>
   </si>
 </sst>
 </file>
@@ -532,15 +553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12295AD0-112B-A740-87F4-84276C9E112C}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +584,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -586,7 +607,7 @@
         <v>1.2761759259259259E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -606,7 +627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -626,7 +647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -646,7 +667,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -662,13 +683,43 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.1308576388888889E-2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -687,8 +738,11 @@
       <c r="F8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G8" s="2">
+        <v>7.7814120370370381E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -702,57 +756,57 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>